<commit_message>
Update missed changes from PA to AA
https://github.com/OWASP/owasp-istg/issues/1
</commit_message>
<xml_diff>
--- a/checklists/checklist.xlsx
+++ b/checklists/checklist.xlsx
@@ -1362,7 +1362,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>IOT-DES-INVAL-001</t>
+          <t>IOT-DES-INPV-001</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1384,7 +1384,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>IOT-DES-INVAL-002</t>
+          <t>IOT-DES-INPV-002</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1626,7 +1626,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>IOT-INT-INVAL-001</t>
+          <t>IOT-INT-INPV-001</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1648,7 +1648,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>IOT-INT-INVAL-002</t>
+          <t>IOT-INT-INPV-002</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -1890,7 +1890,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>IOT-PHY-INVAL-001</t>
+          <t>IOT-PHY-INPV-001</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1912,7 +1912,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>IOT-PHY-INVAL-002</t>
+          <t>IOT-PHY-INPV-002</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -2154,7 +2154,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>IOT-WRLS-INVAL-001</t>
+          <t>IOT-WRLS-INPV-001</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2176,7 +2176,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>IOT-WRLS-INVAL-002</t>
+          <t>IOT-WRLS-INPV-002</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2418,7 +2418,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>IOT-UI-INVAL-001</t>
+          <t>IOT-UI-INPV-001</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2440,7 +2440,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>IOT-UI-INVAL-002</t>
+          <t>IOT-UI-INPV-002</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">

</xml_diff>